<commit_message>
update gebied onbekend en uitrustingsgraad/niveau
</commit_message>
<xml_diff>
--- a/data_voor_swing/aggregatietabellen/arrondiss2018_provincie.xlsx
+++ b/data_voor_swing/aggregatietabellen/arrondiss2018_provincie.xlsx
@@ -382,7 +382,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -401,16 +401,16 @@
       </c>
     </row>
     <row r="2" spans="1:2" s="0" outlineLevel="0">
-      <c r="A2" s="23">
-        <v>11000</v>
+      <c r="A2" s="1" t="e">
+        <v>#NULL!</v>
       </c>
       <c r="B2" s="23">
-        <v>10000</v>
+        <v>99993</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="0" outlineLevel="0">
       <c r="A3" s="23">
-        <v>12000</v>
+        <v>11000</v>
       </c>
       <c r="B3" s="23">
         <v>10000</v>
@@ -418,7 +418,7 @@
     </row>
     <row r="4" spans="1:2" s="0" outlineLevel="0">
       <c r="A4" s="23">
-        <v>13000</v>
+        <v>12000</v>
       </c>
       <c r="B4" s="23">
         <v>10000</v>
@@ -426,23 +426,23 @@
     </row>
     <row r="5" spans="1:2" s="0" outlineLevel="0">
       <c r="A5" s="23">
-        <v>21000</v>
+        <v>13000</v>
       </c>
       <c r="B5" s="23">
-        <v>4000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="6" spans="1:2" s="0" outlineLevel="0">
       <c r="A6" s="23">
-        <v>23000</v>
+        <v>21000</v>
       </c>
       <c r="B6" s="23">
-        <v>20001</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="7" spans="1:2" s="0" outlineLevel="0">
       <c r="A7" s="23">
-        <v>24000</v>
+        <v>23000</v>
       </c>
       <c r="B7" s="23">
         <v>20001</v>
@@ -450,15 +450,15 @@
     </row>
     <row r="8" spans="1:2" s="0" outlineLevel="0">
       <c r="A8" s="23">
-        <v>31000</v>
+        <v>24000</v>
       </c>
       <c r="B8" s="23">
-        <v>30000</v>
+        <v>20001</v>
       </c>
     </row>
     <row r="9" spans="1:2" s="0" outlineLevel="0">
       <c r="A9" s="23">
-        <v>32000</v>
+        <v>31000</v>
       </c>
       <c r="B9" s="23">
         <v>30000</v>
@@ -466,7 +466,7 @@
     </row>
     <row r="10" spans="1:2" s="0" outlineLevel="0">
       <c r="A10" s="23">
-        <v>33000</v>
+        <v>32000</v>
       </c>
       <c r="B10" s="23">
         <v>30000</v>
@@ -474,7 +474,7 @@
     </row>
     <row r="11" spans="1:2" s="0" outlineLevel="0">
       <c r="A11" s="23">
-        <v>34000</v>
+        <v>33000</v>
       </c>
       <c r="B11" s="23">
         <v>30000</v>
@@ -482,7 +482,7 @@
     </row>
     <row r="12" spans="1:2" s="0" outlineLevel="0">
       <c r="A12" s="23">
-        <v>35000</v>
+        <v>34000</v>
       </c>
       <c r="B12" s="23">
         <v>30000</v>
@@ -490,7 +490,7 @@
     </row>
     <row r="13" spans="1:2" s="0" outlineLevel="0">
       <c r="A13" s="23">
-        <v>36000</v>
+        <v>35000</v>
       </c>
       <c r="B13" s="23">
         <v>30000</v>
@@ -498,7 +498,7 @@
     </row>
     <row r="14" spans="1:2" s="0" outlineLevel="0">
       <c r="A14" s="23">
-        <v>37000</v>
+        <v>36000</v>
       </c>
       <c r="B14" s="23">
         <v>30000</v>
@@ -506,7 +506,7 @@
     </row>
     <row r="15" spans="1:2" s="0" outlineLevel="0">
       <c r="A15" s="23">
-        <v>38000</v>
+        <v>37000</v>
       </c>
       <c r="B15" s="23">
         <v>30000</v>
@@ -514,15 +514,15 @@
     </row>
     <row r="16" spans="1:2" s="0" outlineLevel="0">
       <c r="A16" s="23">
-        <v>41000</v>
+        <v>38000</v>
       </c>
       <c r="B16" s="23">
-        <v>40000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="17" spans="1:2" s="0" outlineLevel="0">
       <c r="A17" s="23">
-        <v>42000</v>
+        <v>41000</v>
       </c>
       <c r="B17" s="23">
         <v>40000</v>
@@ -530,7 +530,7 @@
     </row>
     <row r="18" spans="1:2" s="0" outlineLevel="0">
       <c r="A18" s="23">
-        <v>43000</v>
+        <v>42000</v>
       </c>
       <c r="B18" s="23">
         <v>40000</v>
@@ -538,7 +538,7 @@
     </row>
     <row r="19" spans="1:2" s="0" outlineLevel="0">
       <c r="A19" s="23">
-        <v>44000</v>
+        <v>43000</v>
       </c>
       <c r="B19" s="23">
         <v>40000</v>
@@ -546,7 +546,7 @@
     </row>
     <row r="20" spans="1:2" s="0" outlineLevel="0">
       <c r="A20" s="23">
-        <v>45000</v>
+        <v>44000</v>
       </c>
       <c r="B20" s="23">
         <v>40000</v>
@@ -554,7 +554,7 @@
     </row>
     <row r="21" spans="1:2" s="0" outlineLevel="0">
       <c r="A21" s="23">
-        <v>46000</v>
+        <v>45000</v>
       </c>
       <c r="B21" s="23">
         <v>40000</v>
@@ -562,15 +562,15 @@
     </row>
     <row r="22" spans="1:2" s="0" outlineLevel="0">
       <c r="A22" s="23">
-        <v>71000</v>
+        <v>46000</v>
       </c>
       <c r="B22" s="23">
-        <v>70000</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="23" spans="1:2" s="0" outlineLevel="0">
       <c r="A23" s="23">
-        <v>72000</v>
+        <v>71000</v>
       </c>
       <c r="B23" s="23">
         <v>70000</v>
@@ -578,7 +578,7 @@
     </row>
     <row r="24" spans="1:2" s="0" outlineLevel="0">
       <c r="A24" s="23">
-        <v>73000</v>
+        <v>72000</v>
       </c>
       <c r="B24" s="23">
         <v>70000</v>
@@ -586,25 +586,33 @@
     </row>
     <row r="25" spans="1:2" s="0" outlineLevel="0">
       <c r="A25" s="23">
-        <v>99991</v>
+        <v>73000</v>
       </c>
       <c r="B25" s="23">
-        <v>99991</v>
+        <v>70000</v>
       </c>
     </row>
     <row r="26" spans="1:2" s="0" outlineLevel="0">
       <c r="A26" s="23">
-        <v>99992</v>
+        <v>99991</v>
       </c>
       <c r="B26" s="23">
-        <v>4000</v>
+        <v>99991</v>
       </c>
     </row>
     <row r="27" spans="1:2" s="0" outlineLevel="0">
       <c r="A27" s="23">
+        <v>99992</v>
+      </c>
+      <c r="B27" s="23">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" s="0" outlineLevel="0">
+      <c r="A28" s="23">
         <v>99999</v>
       </c>
-      <c r="B27" s="23">
+      <c r="B28" s="23">
         <v>99999</v>
       </c>
     </row>

</xml_diff>